<commit_message>
Updated BOM and added WHO tech spec
</commit_message>
<xml_diff>
--- a/Bill of Materials/Prototype BOM.xlsx
+++ b/Bill of Materials/Prototype BOM.xlsx
@@ -728,8 +728,8 @@
   </sheetPr>
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>